<commit_message>
Letturaok - PART 2.xlsx
</commit_message>
<xml_diff>
--- a/d5/letturaok - PART 2.xlsx
+++ b/d5/letturaok - PART 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5921c20450487a2e/Documents/Compiti-Epicode/d5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{6CB0BA4C-4DEB-459C-ABB7-C7B05811A10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B14BB2A1-21A1-4DBD-810A-7D714E7E7FC9}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{6CB0BA4C-4DEB-459C-ABB7-C7B05811A10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A981DDCC-10FC-4568-A7D6-80B19EB2715F}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{54F1F9A2-5C60-4E81-82D8-03082643D47B}"/>
   </bookViews>
@@ -462,63 +462,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,6 +540,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -836,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B3A704-7E45-47F8-BFE2-78432CF751DA}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -849,268 +858,268 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="21" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>